<commit_message>
fix: correct custom parser registration for TAVIOT_HATZAFON and PASTA_LA_CASA
Changes:
- Fix TAVIOT_HATZAFON parser key to match database code (was TUVIOT with U)
- Update database with customParser: true for both suppliers
- Refactor sober-lerner-parser to use pre-calculated totals from columns G/I
  instead of calculating quantity * commission_per_item
- Update update-all-suppliers.ts script with correct TAVIOT_HATZAFON code

The parsers were not being invoked because:
1. Database lacked customParser: true flag in file_mapping
2. Parser registry used TUVIOT_HATZAFON but database has TAVIOT_HATZAFON

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/raw_data/raw_files_suppliers/קבצים לעמלות רשת/סובר.xlsx
+++ b/raw_data/raw_files_suppliers/קבצים לעמלות רשת/סובר.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arviveli\OneDrive - Chemo Aharon\מסמכים\שולחן העבודה\סטודיו סובר\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D14102E-CD9B-4A12-85B7-ECA863BB2A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAFEE818-012A-4615-8464-65ABDEB58061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{7788A01B-A65F-4D90-803A-4B8AC604040C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7788A01B-A65F-4D90-803A-4B8AC604040C}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -176,9 +176,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא של Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -216,7 +216,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -322,7 +322,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -464,7 +464,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -474,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7534CA91-F6F8-4013-874B-AD3A41F83767}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -529,8 +529,16 @@
       <c r="F3">
         <v>38</v>
       </c>
+      <c r="G3">
+        <f>E3*F3</f>
+        <v>1520</v>
+      </c>
       <c r="H3">
         <v>5</v>
+      </c>
+      <c r="I3">
+        <f>H3*E3</f>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -543,8 +551,16 @@
       <c r="F4">
         <v>53</v>
       </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G25" si="0">E4*F4</f>
+        <v>1060</v>
+      </c>
       <c r="H4">
         <v>5</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I25" si="1">H4*E4</f>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -563,8 +579,16 @@
       <c r="F6">
         <v>38</v>
       </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>2280</v>
+      </c>
       <c r="H6">
         <v>5</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -580,8 +604,16 @@
       <c r="F8">
         <v>72</v>
       </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>936</v>
+      </c>
       <c r="H8">
         <v>4</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -597,7 +629,15 @@
       <c r="F10">
         <v>55</v>
       </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>1100</v>
+      </c>
       <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -617,6 +657,14 @@
       <c r="F13">
         <v>38</v>
       </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>2280</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -631,7 +679,15 @@
       <c r="F15">
         <v>105</v>
       </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>1050</v>
+      </c>
       <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -645,11 +701,19 @@
       <c r="F16">
         <v>72</v>
       </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>1584</v>
+      </c>
       <c r="H16">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>11</v>
       </c>
@@ -659,11 +723,19 @@
       <c r="F17">
         <v>38</v>
       </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>1140</v>
+      </c>
       <c r="H17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>13</v>
       </c>
@@ -673,11 +745,19 @@
       <c r="F18">
         <v>38</v>
       </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>1140</v>
+      </c>
       <c r="H18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>23</v>
       </c>
@@ -687,11 +767,19 @@
       <c r="F19">
         <v>72</v>
       </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>1224</v>
+      </c>
       <c r="H19">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>9</v>
       </c>
@@ -704,11 +792,19 @@
       <c r="F21">
         <v>72</v>
       </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>1224</v>
+      </c>
       <c r="H21">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>25</v>
       </c>
@@ -721,11 +817,19 @@
       <c r="F23">
         <v>72</v>
       </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>1224</v>
+      </c>
       <c r="H23">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>24</v>
       </c>
@@ -738,7 +842,15 @@
       <c r="F25">
         <v>72</v>
       </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>1224</v>
+      </c>
       <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>